<commit_message>
Fixed yet another movement bug.
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -516,7 +516,7 @@
         <v>1</v>
       </c>
       <c t="s" r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="D8">
         <v>1</v>
@@ -575,13 +575,13 @@
         <v>0</v>
       </c>
       <c t="s" r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C9">
         <v>0</v>
       </c>
       <c t="s" r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="E9">
         <v>0</v>
@@ -637,13 +637,13 @@
         <v>0</v>
       </c>
       <c t="s" r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C10">
         <v>0</v>
       </c>
       <c t="s" r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="E10">
         <v>0</v>
@@ -699,13 +699,13 @@
         <v>0</v>
       </c>
       <c t="s" r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C11">
         <v>0</v>
       </c>
       <c t="s" r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="E11">
         <v>0</v>
@@ -761,13 +761,13 @@
         <v>0</v>
       </c>
       <c t="s" r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C12">
         <v>0</v>
       </c>
       <c t="s" r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="E12">
         <v>0</v>
@@ -823,19 +823,19 @@
         <v>0</v>
       </c>
       <c t="s" r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C13">
         <v>0</v>
       </c>
       <c t="s" r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="G13">
         <v>0</v>
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c t="s" r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C14">
         <v>0</v>
@@ -947,19 +947,19 @@
         <v>0</v>
       </c>
       <c t="s" r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" r="G15">
         <v>0</v>

</xml_diff>

<commit_message>
Implemented road, and partially the stoplight. Added more pedestrians, and I am now starting to get the doors to work properly. I will be reorganizing some things.
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -11,12 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="4">
   <si>
     <t>open</t>
   </si>
   <si>
     <t>wall</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>stoplight</t>
   </si>
 </sst>
 </file>
@@ -1130,43 +1136,43 @@
     </row>
     <row r="18">
       <c t="s" r="A18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="B18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="E18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c t="s" r="F18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N18">
         <v>0</v>
@@ -1192,43 +1198,43 @@
     </row>
     <row r="19">
       <c t="s" r="A19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="B19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="C19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="E19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c t="s" r="F19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N19">
         <v>0</v>

</xml_diff>

<commit_message>
Got the basic attract and repel mechanism working. Pathfinding WILL be an issue. In fact, I think there might be an issue with our conceptual model. We'll have to look at this.
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -11,15 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="5">
   <si>
     <t>open</t>
+  </si>
+  <si>
+    <t>road</t>
   </si>
   <si>
     <t>wall</t>
   </si>
   <si>
-    <t>road</t>
+    <t>wall-d</t>
   </si>
   <si>
     <t>stoplight</t>
@@ -139,6 +142,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T1">
+        <v>1</v>
+      </c>
+      <c t="s" r="U1">
+        <v>1</v>
+      </c>
+      <c t="s" r="V1">
+        <v>0</v>
+      </c>
+      <c t="s" r="W1">
+        <v>0</v>
+      </c>
+      <c t="s" r="X1">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y1">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU1">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV1">
         <v>0</v>
       </c>
     </row>
@@ -201,21 +288,105 @@
         <v>0</v>
       </c>
       <c t="s" r="T2">
+        <v>1</v>
+      </c>
+      <c t="s" r="U2">
+        <v>1</v>
+      </c>
+      <c t="s" r="V2">
+        <v>0</v>
+      </c>
+      <c t="s" r="W2">
+        <v>0</v>
+      </c>
+      <c t="s" r="X2">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y2">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU2">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="E3">
         <v>0</v>
@@ -263,57 +434,141 @@
         <v>0</v>
       </c>
       <c t="s" r="T3">
+        <v>1</v>
+      </c>
+      <c t="s" r="U3">
+        <v>1</v>
+      </c>
+      <c t="s" r="V3">
+        <v>0</v>
+      </c>
+      <c t="s" r="W3">
+        <v>0</v>
+      </c>
+      <c t="s" r="X3">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y3">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU3">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV3">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="B4">
         <v>0</v>
       </c>
       <c t="s" r="C4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q4">
         <v>0</v>
@@ -325,57 +580,141 @@
         <v>0</v>
       </c>
       <c t="s" r="T4">
+        <v>1</v>
+      </c>
+      <c t="s" r="U4">
+        <v>1</v>
+      </c>
+      <c t="s" r="V4">
+        <v>0</v>
+      </c>
+      <c t="s" r="W4">
+        <v>0</v>
+      </c>
+      <c t="s" r="X4">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y4">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU4">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV4">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="B5">
         <v>0</v>
       </c>
       <c t="s" r="C5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q5">
         <v>0</v>
@@ -387,57 +726,141 @@
         <v>0</v>
       </c>
       <c t="s" r="T5">
+        <v>1</v>
+      </c>
+      <c t="s" r="U5">
+        <v>1</v>
+      </c>
+      <c t="s" r="V5">
+        <v>0</v>
+      </c>
+      <c t="s" r="W5">
+        <v>0</v>
+      </c>
+      <c t="s" r="X5">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y5">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z5">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA5">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU5">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV5">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="B6">
         <v>0</v>
       </c>
       <c t="s" r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q6">
         <v>0</v>
@@ -449,57 +872,141 @@
         <v>0</v>
       </c>
       <c t="s" r="T6">
+        <v>1</v>
+      </c>
+      <c t="s" r="U6">
+        <v>1</v>
+      </c>
+      <c t="s" r="V6">
+        <v>0</v>
+      </c>
+      <c t="s" r="W6">
+        <v>0</v>
+      </c>
+      <c t="s" r="X6">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y6">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z6">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA6">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU6">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV6">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="B7">
         <v>0</v>
       </c>
       <c t="s" r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q7">
         <v>0</v>
@@ -511,57 +1018,141 @@
         <v>0</v>
       </c>
       <c t="s" r="T7">
+        <v>1</v>
+      </c>
+      <c t="s" r="U7">
+        <v>1</v>
+      </c>
+      <c t="s" r="V7">
+        <v>0</v>
+      </c>
+      <c t="s" r="W7">
+        <v>0</v>
+      </c>
+      <c t="s" r="X7">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y7">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z7">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA7">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU7">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV7">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q8">
         <v>0</v>
@@ -573,6 +1164,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T8">
+        <v>1</v>
+      </c>
+      <c t="s" r="U8">
+        <v>1</v>
+      </c>
+      <c t="s" r="V8">
+        <v>0</v>
+      </c>
+      <c t="s" r="W8">
+        <v>0</v>
+      </c>
+      <c t="s" r="X8">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y8">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z8">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA8">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU8">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV8">
         <v>0</v>
       </c>
     </row>
@@ -581,49 +1256,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q9">
         <v>0</v>
@@ -635,6 +1310,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T9">
+        <v>1</v>
+      </c>
+      <c t="s" r="U9">
+        <v>1</v>
+      </c>
+      <c t="s" r="V9">
+        <v>0</v>
+      </c>
+      <c t="s" r="W9">
+        <v>0</v>
+      </c>
+      <c t="s" r="X9">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y9">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z9">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA9">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU9">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV9">
         <v>0</v>
       </c>
     </row>
@@ -643,49 +1402,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q10">
         <v>0</v>
@@ -697,6 +1456,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T10">
+        <v>1</v>
+      </c>
+      <c t="s" r="U10">
+        <v>1</v>
+      </c>
+      <c t="s" r="V10">
+        <v>0</v>
+      </c>
+      <c t="s" r="W10">
+        <v>0</v>
+      </c>
+      <c t="s" r="X10">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y10">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z10">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA10">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU10">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV10">
         <v>0</v>
       </c>
     </row>
@@ -705,49 +1548,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c t="s" r="Q11">
         <v>0</v>
@@ -759,6 +1602,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T11">
+        <v>4</v>
+      </c>
+      <c t="s" r="U11">
+        <v>4</v>
+      </c>
+      <c t="s" r="V11">
+        <v>0</v>
+      </c>
+      <c t="s" r="W11">
+        <v>0</v>
+      </c>
+      <c t="s" r="X11">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y11">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z11">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA11">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU11">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV11">
         <v>0</v>
       </c>
     </row>
@@ -767,49 +1694,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q12">
         <v>0</v>
@@ -821,6 +1748,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T12">
+        <v>1</v>
+      </c>
+      <c t="s" r="U12">
+        <v>1</v>
+      </c>
+      <c t="s" r="V12">
+        <v>0</v>
+      </c>
+      <c t="s" r="W12">
+        <v>0</v>
+      </c>
+      <c t="s" r="X12">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y12">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z12">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA12">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU12">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV12">
         <v>0</v>
       </c>
     </row>
@@ -829,49 +1840,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="G13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q13">
         <v>0</v>
@@ -883,6 +1894,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T13">
+        <v>1</v>
+      </c>
+      <c t="s" r="U13">
+        <v>1</v>
+      </c>
+      <c t="s" r="V13">
+        <v>0</v>
+      </c>
+      <c t="s" r="W13">
+        <v>0</v>
+      </c>
+      <c t="s" r="X13">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y13">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z13">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA13">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU13">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV13">
         <v>0</v>
       </c>
     </row>
@@ -891,49 +1986,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="E14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q14">
         <v>0</v>
@@ -945,6 +2040,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T14">
+        <v>1</v>
+      </c>
+      <c t="s" r="U14">
+        <v>1</v>
+      </c>
+      <c t="s" r="V14">
+        <v>0</v>
+      </c>
+      <c t="s" r="W14">
+        <v>0</v>
+      </c>
+      <c t="s" r="X14">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y14">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z14">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA14">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU14">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV14">
         <v>0</v>
       </c>
     </row>
@@ -953,49 +2132,49 @@
         <v>0</v>
       </c>
       <c t="s" r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c t="s" r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" r="G15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q15">
         <v>0</v>
@@ -1007,6 +2186,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T15">
+        <v>1</v>
+      </c>
+      <c t="s" r="U15">
+        <v>1</v>
+      </c>
+      <c t="s" r="V15">
+        <v>0</v>
+      </c>
+      <c t="s" r="W15">
+        <v>0</v>
+      </c>
+      <c t="s" r="X15">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y15">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z15">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA15">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU15">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV15">
         <v>0</v>
       </c>
     </row>
@@ -1018,46 +2281,46 @@
         <v>0</v>
       </c>
       <c t="s" r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q16">
         <v>0</v>
@@ -1069,6 +2332,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T16">
+        <v>1</v>
+      </c>
+      <c t="s" r="U16">
+        <v>1</v>
+      </c>
+      <c t="s" r="V16">
+        <v>0</v>
+      </c>
+      <c t="s" r="W16">
+        <v>0</v>
+      </c>
+      <c t="s" r="X16">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y16">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z16">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA16">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU16">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV16">
         <v>0</v>
       </c>
     </row>
@@ -1080,46 +2427,46 @@
         <v>0</v>
       </c>
       <c t="s" r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="E17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="G17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="H17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="I17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="J17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q17">
         <v>0</v>
@@ -1131,15 +2478,99 @@
         <v>0</v>
       </c>
       <c t="s" r="T17">
+        <v>1</v>
+      </c>
+      <c t="s" r="U17">
+        <v>1</v>
+      </c>
+      <c t="s" r="V17">
+        <v>0</v>
+      </c>
+      <c t="s" r="W17">
+        <v>0</v>
+      </c>
+      <c t="s" r="X17">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y17">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z17">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA17">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU17">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV17">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c t="s" r="A18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="B18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="C18">
         <v>2</v>
@@ -1148,7 +2579,7 @@
         <v>2</v>
       </c>
       <c t="s" r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c t="s" r="F18">
         <v>2</v>
@@ -1175,13 +2606,13 @@
         <v>2</v>
       </c>
       <c t="s" r="N18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q18">
         <v>0</v>
@@ -1193,36 +2624,120 @@
         <v>0</v>
       </c>
       <c t="s" r="T18">
+        <v>1</v>
+      </c>
+      <c t="s" r="U18">
+        <v>1</v>
+      </c>
+      <c t="s" r="V18">
+        <v>0</v>
+      </c>
+      <c t="s" r="W18">
+        <v>0</v>
+      </c>
+      <c t="s" r="X18">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y18">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z18">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA18">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU18">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV18">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c t="s" r="A19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="B19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="D19">
         <v>2</v>
       </c>
       <c t="s" r="E19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c t="s" r="F19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="G19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="H19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="I19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c t="s" r="J19">
         <v>2</v>
@@ -1237,13 +2752,13 @@
         <v>2</v>
       </c>
       <c t="s" r="N19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q19">
         <v>0</v>
@@ -1255,6 +2770,90 @@
         <v>0</v>
       </c>
       <c t="s" r="T19">
+        <v>1</v>
+      </c>
+      <c t="s" r="U19">
+        <v>1</v>
+      </c>
+      <c t="s" r="V19">
+        <v>0</v>
+      </c>
+      <c t="s" r="W19">
+        <v>0</v>
+      </c>
+      <c t="s" r="X19">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y19">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z19">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA19">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU19">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV19">
         <v>0</v>
       </c>
     </row>
@@ -1269,10 +2868,10 @@
         <v>0</v>
       </c>
       <c t="s" r="D20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="E20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="F20">
         <v>0</v>
@@ -1287,25 +2886,25 @@
         <v>0</v>
       </c>
       <c t="s" r="J20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="K20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="L20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="M20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="N20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="O20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="P20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c t="s" r="Q20">
         <v>0</v>
@@ -1317,6 +2916,820 @@
         <v>0</v>
       </c>
       <c t="s" r="T20">
+        <v>1</v>
+      </c>
+      <c t="s" r="U20">
+        <v>1</v>
+      </c>
+      <c t="s" r="V20">
+        <v>0</v>
+      </c>
+      <c t="s" r="W20">
+        <v>0</v>
+      </c>
+      <c t="s" r="X20">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y20">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z20">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA20">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU20">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" r="A21">
+        <v>0</v>
+      </c>
+      <c t="s" r="B21">
+        <v>0</v>
+      </c>
+      <c t="s" r="C21">
+        <v>0</v>
+      </c>
+      <c t="s" r="D21">
+        <v>0</v>
+      </c>
+      <c t="s" r="E21">
+        <v>0</v>
+      </c>
+      <c t="s" r="F21">
+        <v>0</v>
+      </c>
+      <c t="s" r="G21">
+        <v>0</v>
+      </c>
+      <c t="s" r="H21">
+        <v>0</v>
+      </c>
+      <c t="s" r="I21">
+        <v>0</v>
+      </c>
+      <c t="s" r="J21">
+        <v>2</v>
+      </c>
+      <c t="s" r="K21">
+        <v>2</v>
+      </c>
+      <c t="s" r="L21">
+        <v>2</v>
+      </c>
+      <c t="s" r="M21">
+        <v>2</v>
+      </c>
+      <c t="s" r="N21">
+        <v>2</v>
+      </c>
+      <c t="s" r="O21">
+        <v>2</v>
+      </c>
+      <c t="s" r="P21">
+        <v>2</v>
+      </c>
+      <c t="s" r="Q21">
+        <v>0</v>
+      </c>
+      <c t="s" r="R21">
+        <v>0</v>
+      </c>
+      <c t="s" r="S21">
+        <v>0</v>
+      </c>
+      <c t="s" r="T21">
+        <v>1</v>
+      </c>
+      <c t="s" r="U21">
+        <v>1</v>
+      </c>
+      <c t="s" r="V21">
+        <v>0</v>
+      </c>
+      <c t="s" r="W21">
+        <v>0</v>
+      </c>
+      <c t="s" r="X21">
+        <v>2</v>
+      </c>
+      <c t="s" r="Y21">
+        <v>2</v>
+      </c>
+      <c t="s" r="Z21">
+        <v>2</v>
+      </c>
+      <c t="s" r="AA21">
+        <v>2</v>
+      </c>
+      <c t="s" r="AB21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU21">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" r="A22">
+        <v>0</v>
+      </c>
+      <c t="s" r="B22">
+        <v>0</v>
+      </c>
+      <c t="s" r="C22">
+        <v>0</v>
+      </c>
+      <c t="s" r="D22">
+        <v>0</v>
+      </c>
+      <c t="s" r="E22">
+        <v>0</v>
+      </c>
+      <c t="s" r="F22">
+        <v>0</v>
+      </c>
+      <c t="s" r="G22">
+        <v>0</v>
+      </c>
+      <c t="s" r="H22">
+        <v>0</v>
+      </c>
+      <c t="s" r="I22">
+        <v>0</v>
+      </c>
+      <c t="s" r="J22">
+        <v>2</v>
+      </c>
+      <c t="s" r="K22">
+        <v>2</v>
+      </c>
+      <c t="s" r="L22">
+        <v>2</v>
+      </c>
+      <c t="s" r="M22">
+        <v>2</v>
+      </c>
+      <c t="s" r="N22">
+        <v>2</v>
+      </c>
+      <c t="s" r="O22">
+        <v>0</v>
+      </c>
+      <c t="s" r="P22">
+        <v>0</v>
+      </c>
+      <c t="s" r="Q22">
+        <v>0</v>
+      </c>
+      <c t="s" r="R22">
+        <v>0</v>
+      </c>
+      <c t="s" r="S22">
+        <v>0</v>
+      </c>
+      <c t="s" r="T22">
+        <v>1</v>
+      </c>
+      <c t="s" r="U22">
+        <v>1</v>
+      </c>
+      <c t="s" r="V22">
+        <v>0</v>
+      </c>
+      <c t="s" r="W22">
+        <v>0</v>
+      </c>
+      <c t="s" r="X22">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y22">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU22">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" r="A23">
+        <v>0</v>
+      </c>
+      <c t="s" r="B23">
+        <v>0</v>
+      </c>
+      <c t="s" r="C23">
+        <v>0</v>
+      </c>
+      <c t="s" r="D23">
+        <v>0</v>
+      </c>
+      <c t="s" r="E23">
+        <v>0</v>
+      </c>
+      <c t="s" r="F23">
+        <v>0</v>
+      </c>
+      <c t="s" r="G23">
+        <v>0</v>
+      </c>
+      <c t="s" r="H23">
+        <v>0</v>
+      </c>
+      <c t="s" r="I23">
+        <v>0</v>
+      </c>
+      <c t="s" r="J23">
+        <v>0</v>
+      </c>
+      <c t="s" r="K23">
+        <v>0</v>
+      </c>
+      <c t="s" r="L23">
+        <v>0</v>
+      </c>
+      <c t="s" r="M23">
+        <v>0</v>
+      </c>
+      <c t="s" r="N23">
+        <v>0</v>
+      </c>
+      <c t="s" r="O23">
+        <v>0</v>
+      </c>
+      <c t="s" r="P23">
+        <v>0</v>
+      </c>
+      <c t="s" r="Q23">
+        <v>0</v>
+      </c>
+      <c t="s" r="R23">
+        <v>0</v>
+      </c>
+      <c t="s" r="S23">
+        <v>0</v>
+      </c>
+      <c t="s" r="T23">
+        <v>1</v>
+      </c>
+      <c t="s" r="U23">
+        <v>1</v>
+      </c>
+      <c t="s" r="V23">
+        <v>0</v>
+      </c>
+      <c t="s" r="W23">
+        <v>0</v>
+      </c>
+      <c t="s" r="X23">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y23">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU23">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" r="A24">
+        <v>0</v>
+      </c>
+      <c t="s" r="B24">
+        <v>0</v>
+      </c>
+      <c t="s" r="C24">
+        <v>0</v>
+      </c>
+      <c t="s" r="D24">
+        <v>0</v>
+      </c>
+      <c t="s" r="E24">
+        <v>0</v>
+      </c>
+      <c t="s" r="F24">
+        <v>0</v>
+      </c>
+      <c t="s" r="G24">
+        <v>0</v>
+      </c>
+      <c t="s" r="H24">
+        <v>0</v>
+      </c>
+      <c t="s" r="I24">
+        <v>0</v>
+      </c>
+      <c t="s" r="J24">
+        <v>0</v>
+      </c>
+      <c t="s" r="K24">
+        <v>0</v>
+      </c>
+      <c t="s" r="L24">
+        <v>0</v>
+      </c>
+      <c t="s" r="M24">
+        <v>0</v>
+      </c>
+      <c t="s" r="N24">
+        <v>0</v>
+      </c>
+      <c t="s" r="O24">
+        <v>0</v>
+      </c>
+      <c t="s" r="P24">
+        <v>0</v>
+      </c>
+      <c t="s" r="Q24">
+        <v>0</v>
+      </c>
+      <c t="s" r="R24">
+        <v>0</v>
+      </c>
+      <c t="s" r="S24">
+        <v>0</v>
+      </c>
+      <c t="s" r="T24">
+        <v>1</v>
+      </c>
+      <c t="s" r="U24">
+        <v>1</v>
+      </c>
+      <c t="s" r="V24">
+        <v>0</v>
+      </c>
+      <c t="s" r="W24">
+        <v>0</v>
+      </c>
+      <c t="s" r="X24">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y24">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU24">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" r="A25">
+        <v>0</v>
+      </c>
+      <c t="s" r="B25">
+        <v>0</v>
+      </c>
+      <c t="s" r="C25">
+        <v>0</v>
+      </c>
+      <c t="s" r="D25">
+        <v>0</v>
+      </c>
+      <c t="s" r="E25">
+        <v>0</v>
+      </c>
+      <c t="s" r="F25">
+        <v>0</v>
+      </c>
+      <c t="s" r="G25">
+        <v>0</v>
+      </c>
+      <c t="s" r="H25">
+        <v>0</v>
+      </c>
+      <c t="s" r="I25">
+        <v>0</v>
+      </c>
+      <c t="s" r="J25">
+        <v>0</v>
+      </c>
+      <c t="s" r="K25">
+        <v>0</v>
+      </c>
+      <c t="s" r="L25">
+        <v>0</v>
+      </c>
+      <c t="s" r="M25">
+        <v>0</v>
+      </c>
+      <c t="s" r="N25">
+        <v>0</v>
+      </c>
+      <c t="s" r="O25">
+        <v>0</v>
+      </c>
+      <c t="s" r="P25">
+        <v>0</v>
+      </c>
+      <c t="s" r="Q25">
+        <v>0</v>
+      </c>
+      <c t="s" r="R25">
+        <v>0</v>
+      </c>
+      <c t="s" r="S25">
+        <v>0</v>
+      </c>
+      <c t="s" r="T25">
+        <v>1</v>
+      </c>
+      <c t="s" r="U25">
+        <v>1</v>
+      </c>
+      <c t="s" r="V25">
+        <v>0</v>
+      </c>
+      <c t="s" r="W25">
+        <v>0</v>
+      </c>
+      <c t="s" r="X25">
+        <v>0</v>
+      </c>
+      <c t="s" r="Y25">
+        <v>0</v>
+      </c>
+      <c t="s" r="Z25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AA25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AB25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AC25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AD25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AE25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AF25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AG25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AH25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AI25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AJ25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AK25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AL25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AM25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AN25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AO25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AP25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AQ25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AR25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AS25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AT25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AU25">
+        <v>0</v>
+      </c>
+      <c t="s" r="AV25">
         <v>0</v>
       </c>
     </row>

</xml_diff>